<commit_message>
added new acceptable excel format
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
-  <workbookPr/>
+  <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rrosales/Documents/nodeproj/excelparse/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2720" windowWidth="25600" windowHeight="11820"/>
+    <workbookView xWindow="32560" yWindow="1820" windowWidth="26980" windowHeight="15800"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,28 +30,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Campaign ID</t>
   </si>
   <si>
-    <t>Impression URL</t>
-  </si>
-  <si>
-    <t>google.com</t>
-  </si>
-  <si>
-    <t>yahoo.com</t>
-  </si>
-  <si>
-    <t>&lt;IMG SRC="ttteeessttturl.com" BORDER="0" HEIGHT="1" WIDTH="1" ALT="Advertisement"&gt;</t>
+    <t>Campaign Name</t>
+  </si>
+  <si>
+    <t>Impression tags</t>
+  </si>
+  <si>
+    <t>&lt;A HREF="https://ad.doubleclick.net/ddm/jump/N5214.1984505OUTBRAIN/B10820811.144578431;sz=1x1;ord=[timestamp]?"&gt;
+&lt;IMG SRC="https://ad.doubleclick.net/ddm/ad/N5214.1984505OUTBRAIN/B10820811.144578431;sz=1x1;ord=[timestamp];dc_lat=;dc_rdid=;tag_for_child_directed_treatment=?" BORDER=0 WIDTH=1 HEIGHT=1 ALT="Advertisement"&gt;&lt;/A&gt;</t>
+  </si>
+  <si>
+    <t>&lt;A HREF="https://ad.doubleclick.net/ddm/jump/N5214.1984505OUTBRAIN/B10822178.144574948;sz=1x1;ord=[timestamp]?"&gt;
+&lt;IMG SRC="https://ad.doubleclick.net/ddm/ad/N5214.1984505OUTBRAIN/B10822178.144574948;sz=1x1;ord=[timestamp];dc_lat=;dc_rdid=;tag_for_child_directed_treatment=?" BORDER=0 WIDTH=1 HEIGHT=1 ALT="Advertisement"&gt;&lt;/A&gt;</t>
+  </si>
+  <si>
+    <t>&lt;A HREF="https://ad.doubleclick.net/ddm/jump/N5214.1984505OUTBRAIN/B10821032.144577266;sz=1x1;ord=[timestamp]?"&gt;
+&lt;IMG SRC="https://ad.doubleclick.net/ddm/ad/N5214.1984505OUTBRAIN/B10821032.144577266;sz=1x1;ord=[timestamp];dc_lat=;dc_rdid=;tag_for_child_directed_treatment=?" BORDER=0 WIDTH=1 HEIGHT=1 ALT="Advertisement"&gt;&lt;/A&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img src='http://stackoverflow.com/questions/154059/how-do-you-check-for-an-empty-string-in-javascript'&gt;&lt;/img&gt;</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/17238144/string-check-with-if-js-shorthand?noredirect=1&amp;lq=1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,24 +75,67 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -85,20 +143,69 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="8">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -156,7 +263,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -208,7 +315,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -410,111 +517,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="143.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="143.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1000328717</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
+    <row r="2" spans="1:3" ht="33" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1000346945</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1000328717</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="1:3" ht="33" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>1000346948</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1000328717</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
+    <row r="4" spans="1:3" ht="33" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>1000346949</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1000328722</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>10003422249</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>1000328726</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>1000328728</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>1000328737</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>1000328738</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>1000328739</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>4</v>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>10346949</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
 </file>
</xml_diff>